<commit_message>
minor cleanup - TRY_analysis and test_solvents
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/HP/analyses/HP_2021.7.29-0.59_0_baseline.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/HP/analyses/HP_2021.7.29-0.59_0_baseline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\BioSTEAM 2.x.x\biorefineries\HP\analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216A4FFD-7A82-40A9-985F-ABCD6DE320DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E6D62B-8341-4722-A439-4B68D22CF682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -566,14 +566,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -914,137 +914,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DL37"/>
+  <dimension ref="A1:DL30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O16" workbookViewId="0">
-      <selection activeCell="W32" sqref="W32"/>
+    <sheetView tabSelected="1" topLeftCell="BV3" workbookViewId="0">
+      <selection activeCell="CH14" sqref="CH14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
-      <c r="AG1" s="15"/>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="15"/>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="15"/>
-      <c r="AN1" s="15"/>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="15"/>
-      <c r="AQ1" s="15"/>
-      <c r="AR1" s="15"/>
-      <c r="AS1" s="15"/>
-      <c r="AT1" s="15"/>
-      <c r="AU1" s="15"/>
-      <c r="AV1" s="15"/>
-      <c r="AW1" s="15"/>
-      <c r="AX1" s="15"/>
-      <c r="AY1" s="15"/>
-      <c r="AZ1" s="15"/>
-      <c r="BA1" s="15"/>
-      <c r="BB1" s="15"/>
-      <c r="BC1" s="15"/>
-      <c r="BD1" s="15"/>
-      <c r="BE1" s="15"/>
-      <c r="BF1" s="15" t="s">
+      <c r="B1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
+      <c r="AD1" s="17"/>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="17"/>
+      <c r="AG1" s="17"/>
+      <c r="AH1" s="17"/>
+      <c r="AI1" s="17"/>
+      <c r="AJ1" s="17"/>
+      <c r="AK1" s="17"/>
+      <c r="AL1" s="17"/>
+      <c r="AM1" s="17"/>
+      <c r="AN1" s="17"/>
+      <c r="AO1" s="17"/>
+      <c r="AP1" s="17"/>
+      <c r="AQ1" s="17"/>
+      <c r="AR1" s="17"/>
+      <c r="AS1" s="17"/>
+      <c r="AT1" s="17"/>
+      <c r="AU1" s="17"/>
+      <c r="AV1" s="17"/>
+      <c r="AW1" s="17"/>
+      <c r="AX1" s="17"/>
+      <c r="AY1" s="17"/>
+      <c r="AZ1" s="17"/>
+      <c r="BA1" s="17"/>
+      <c r="BB1" s="17"/>
+      <c r="BC1" s="17"/>
+      <c r="BD1" s="17"/>
+      <c r="BE1" s="17"/>
+      <c r="BF1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="BG1" s="15"/>
-      <c r="BH1" s="15"/>
-      <c r="BI1" s="15"/>
-      <c r="BJ1" s="15"/>
-      <c r="BK1" s="15"/>
-      <c r="BL1" s="15"/>
-      <c r="BM1" s="15"/>
-      <c r="BN1" s="15"/>
-      <c r="BO1" s="15"/>
-      <c r="BP1" s="15"/>
-      <c r="BQ1" s="15"/>
-      <c r="BR1" s="15"/>
-      <c r="BS1" s="15"/>
-      <c r="BT1" s="15" t="s">
+      <c r="BG1" s="17"/>
+      <c r="BH1" s="17"/>
+      <c r="BI1" s="17"/>
+      <c r="BJ1" s="17"/>
+      <c r="BK1" s="17"/>
+      <c r="BL1" s="17"/>
+      <c r="BM1" s="17"/>
+      <c r="BN1" s="17"/>
+      <c r="BO1" s="17"/>
+      <c r="BP1" s="17"/>
+      <c r="BQ1" s="17"/>
+      <c r="BR1" s="17"/>
+      <c r="BS1" s="17"/>
+      <c r="BT1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="BU1" s="15"/>
-      <c r="BV1" s="15"/>
-      <c r="BW1" s="15"/>
-      <c r="BX1" s="15" t="s">
+      <c r="BU1" s="17"/>
+      <c r="BV1" s="17"/>
+      <c r="BW1" s="17"/>
+      <c r="BX1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="BY1" s="15"/>
-      <c r="BZ1" s="15" t="s">
+      <c r="BY1" s="17"/>
+      <c r="BZ1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="CA1" s="15"/>
-      <c r="CB1" s="15"/>
-      <c r="CC1" s="15"/>
-      <c r="CD1" s="15"/>
-      <c r="CE1" s="15"/>
-      <c r="CF1" s="15"/>
-      <c r="CG1" s="15"/>
-      <c r="CH1" s="15"/>
-      <c r="CI1" s="15"/>
-      <c r="CJ1" s="15"/>
-      <c r="CK1" s="15"/>
-      <c r="CL1" s="15"/>
-      <c r="CM1" s="15"/>
-      <c r="CN1" s="15"/>
-      <c r="CO1" s="15"/>
-      <c r="CP1" s="15"/>
-      <c r="CQ1" s="15"/>
-      <c r="CR1" s="15"/>
-      <c r="CS1" s="15"/>
-      <c r="CT1" s="15"/>
-      <c r="CU1" s="15"/>
-      <c r="CV1" s="15"/>
-      <c r="CW1" s="15"/>
-      <c r="CX1" s="15"/>
-      <c r="CY1" s="15"/>
-      <c r="CZ1" s="15"/>
-      <c r="DA1" s="15"/>
-      <c r="DB1" s="15"/>
-      <c r="DC1" s="15"/>
-      <c r="DD1" s="15"/>
-      <c r="DE1" s="15"/>
-      <c r="DF1" s="15"/>
-      <c r="DG1" s="15"/>
-      <c r="DH1" s="15"/>
+      <c r="CA1" s="17"/>
+      <c r="CB1" s="17"/>
+      <c r="CC1" s="17"/>
+      <c r="CD1" s="17"/>
+      <c r="CE1" s="17"/>
+      <c r="CF1" s="17"/>
+      <c r="CG1" s="17"/>
+      <c r="CH1" s="17"/>
+      <c r="CI1" s="17"/>
+      <c r="CJ1" s="17"/>
+      <c r="CK1" s="17"/>
+      <c r="CL1" s="17"/>
+      <c r="CM1" s="17"/>
+      <c r="CN1" s="17"/>
+      <c r="CO1" s="17"/>
+      <c r="CP1" s="17"/>
+      <c r="CQ1" s="17"/>
+      <c r="CR1" s="17"/>
+      <c r="CS1" s="17"/>
+      <c r="CT1" s="17"/>
+      <c r="CU1" s="17"/>
+      <c r="CV1" s="17"/>
+      <c r="CW1" s="17"/>
+      <c r="CX1" s="17"/>
+      <c r="CY1" s="17"/>
+      <c r="CZ1" s="17"/>
+      <c r="DA1" s="17"/>
+      <c r="DB1" s="17"/>
+      <c r="DC1" s="17"/>
+      <c r="DD1" s="17"/>
+      <c r="DE1" s="17"/>
+      <c r="DF1" s="17"/>
+      <c r="DG1" s="17"/>
+      <c r="DH1" s="17"/>
     </row>
     <row r="2" spans="1:116" s="14" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
@@ -2217,8 +2217,20 @@
         <v>134</v>
       </c>
     </row>
+    <row r="16" spans="1:116" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="15"/>
+      <c r="CI16" s="7"/>
+      <c r="CQ16" s="7"/>
+      <c r="CR16" s="8"/>
+      <c r="CS16" s="7"/>
+      <c r="CT16" s="9"/>
+      <c r="CU16" s="9"/>
+      <c r="CV16" s="7"/>
+      <c r="CW16" s="9"/>
+      <c r="CX16" s="9"/>
+    </row>
     <row r="17" spans="1:116" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
+      <c r="A17" s="15"/>
       <c r="K17" s="6">
         <f>R5/(SUM($M5:$U5)-$S5-$R5)</f>
         <v>-0.28769215019410566</v>
@@ -2444,7 +2456,7 @@
         <v>2.8075663055698752E-2</v>
       </c>
       <c r="CE17" s="6">
-        <f t="shared" si="7"/>
+        <f>CE5/$BZ5</f>
         <v>0.16798010531072058</v>
       </c>
       <c r="CF17" s="6">
@@ -2557,7 +2569,7 @@
       </c>
     </row>
     <row r="27" spans="1:116" s="5" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="M27" s="17" t="s">
+      <c r="M27" s="16" t="s">
         <v>138</v>
       </c>
       <c r="N27" s="5">
@@ -2572,7 +2584,7 @@
         <f>P17/SUM(M17:Q17)</f>
         <v>0.76013380025728194</v>
       </c>
-      <c r="V27" s="17" t="s">
+      <c r="V27" s="16" t="s">
         <v>139</v>
       </c>
       <c r="W27" s="5">
@@ -2616,11 +2628,6 @@
       <c r="CU30" s="12"/>
       <c r="CW30" s="12"/>
     </row>
-    <row r="33" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="37" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B1:BE1"/>

</xml_diff>